<commit_message>
Added new images of camera 2 for testing.
</commit_message>
<xml_diff>
--- a/graphics.xlsx
+++ b/graphics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\opt\windows\Microsoft\VisualStudio\repos\CameraCalibration\QtFrontoParallel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9040ACF7-AD7E-4ACD-B52D-632DF591683D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C03AC03-1424-4A69-A989-631DEB058806}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5568" xr2:uid="{DFD5A370-DE3D-47F8-981C-568D4120CDD8}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5568" activeTab="1" xr2:uid="{DFD5A370-DE3D-47F8-981C-568D4120CDD8}"/>
   </bookViews>
   <sheets>
     <sheet name="cam1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="7">
   <si>
     <t>id</t>
   </si>
@@ -1196,6 +1196,1095 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-PE"/>
+              <a:t>RMS vs Iteration</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-PE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'cam2'!$G$2:$G$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>0.37133899999999997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.36565399999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.36426900000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.363541</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.36338500000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.36272500000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.36281799999999997</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.36292000000000002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.36304599999999998</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.36258400000000002</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.36273499999999997</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.36260399999999998</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.36316999999999999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.36301899999999998</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.36296499999999998</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.36278899999999997</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.36255300000000001</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.36227199999999998</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.36220599999999997</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.36219899999999999</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.36247299999999999</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.36206500000000003</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.36268400000000001</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.36233399999999999</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.36259599999999997</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.36243900000000001</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.36257499999999998</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.36272399999999999</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.36263499999999999</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.362514</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4F1E-4E5A-9DF7-A5DD85636CD8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="345197152"/>
+        <c:axId val="345198136"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="345197152"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-PE"/>
+                  <a:t>Iterations</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-PE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-PE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="345198136"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="345198136"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-PE"/>
+                  <a:t>RMS</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-PE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-PE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="345197152"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-PE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-PE"/>
+              <a:t>Center</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="es-PE" baseline="0"/>
+              <a:t> of Image</a:t>
+            </a:r>
+            <a:endParaRPr lang="es-PE"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.38798600174978126"/>
+          <c:y val="2.3148148148148147E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-PE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'cam2'!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Cy</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'cam2'!$E$2:$E$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>343.37299999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>343.40499999999997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>343.548</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>343.488</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>343.49599999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>343.51799999999997</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>343.512</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>343.62599999999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>343.63200000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>343.57400000000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>343.529</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>343.51</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>343.52600000000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>343.50099999999998</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>343.47300000000001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>343.49700000000001</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>343.61399999999998</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>343.51400000000001</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>343.52100000000002</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>343.55500000000001</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>343.51299999999998</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>343.57400000000001</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>343.541</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>343.584</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>343.60599999999999</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>343.529</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>343.59100000000001</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>343.57799999999997</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>343.54899999999998</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>343.49299999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'cam2'!$F$2:$F$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>176.05199999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>175.98699999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>175.976</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>176.02</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>175.99700000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>176.09700000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>176.07499999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>176.06299999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>175.96899999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>175.941</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>175.90299999999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>175.92699999999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>175.87</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>176.04499999999999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>175.876</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>175.93600000000001</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>176.02600000000001</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>175.87899999999999</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>175.91300000000001</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>175.989</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>175.953</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>175.899</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>175.91499999999999</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>175.995</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>175.98099999999999</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>175.88900000000001</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>175.90199999999999</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>175.94499999999999</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>175.80099999999999</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>175.797</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-CD71-4F4C-B209-48801A847CBE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="524262256"/>
+        <c:axId val="524264224"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="524262256"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-PE"/>
+                  <a:t>Cx</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-PE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="low"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-PE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="524264224"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="524264224"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-PE"/>
+                  <a:t>Cy</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-PE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-PE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="524262256"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-PE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1276,6 +2365,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -1793,6 +2962,1038 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2369,6 +4570,87 @@
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7FA8F0C1-14BC-49D8-B441-B8F1E9875ED9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Gráfico 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{19EAEF79-FE2A-47C8-9916-440ABA23E10D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -2684,8 +4966,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45452647-02B4-4D77-B9D7-AC0F3928746E}">
   <dimension ref="B1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="Q21" sqref="Q21"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="H1" sqref="B1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3411,12 +5693,729 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D45F17D-AD8D-463A-9C71-31EA20C98AB7}">
-  <dimension ref="A1"/>
+  <dimension ref="B1:H31"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P24" sqref="P24"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>475.767</v>
+      </c>
+      <c r="D2">
+        <v>476.19</v>
+      </c>
+      <c r="E2">
+        <v>343.37299999999999</v>
+      </c>
+      <c r="F2">
+        <v>176.05199999999999</v>
+      </c>
+      <c r="G2">
+        <v>0.37133899999999997</v>
+      </c>
+      <c r="H2">
+        <v>4.5352799999999999E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>475.36</v>
+      </c>
+      <c r="D3">
+        <v>475.75299999999999</v>
+      </c>
+      <c r="E3">
+        <v>343.40499999999997</v>
+      </c>
+      <c r="F3">
+        <v>175.98699999999999</v>
+      </c>
+      <c r="G3">
+        <v>0.36565399999999998</v>
+      </c>
+      <c r="H3">
+        <v>3.5694700000000003E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>475.233</v>
+      </c>
+      <c r="D4">
+        <v>475.60199999999998</v>
+      </c>
+      <c r="E4">
+        <v>343.548</v>
+      </c>
+      <c r="F4">
+        <v>175.976</v>
+      </c>
+      <c r="G4">
+        <v>0.36426900000000001</v>
+      </c>
+      <c r="H4">
+        <v>3.3199600000000003E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>475.20699999999999</v>
+      </c>
+      <c r="D5">
+        <v>475.55900000000003</v>
+      </c>
+      <c r="E5">
+        <v>343.488</v>
+      </c>
+      <c r="F5">
+        <v>176.02</v>
+      </c>
+      <c r="G5">
+        <v>0.363541</v>
+      </c>
+      <c r="H5">
+        <v>3.2205299999999999E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>475.20699999999999</v>
+      </c>
+      <c r="D6">
+        <v>475.56</v>
+      </c>
+      <c r="E6">
+        <v>343.49599999999998</v>
+      </c>
+      <c r="F6">
+        <v>175.99700000000001</v>
+      </c>
+      <c r="G6">
+        <v>0.36338500000000001</v>
+      </c>
+      <c r="H6">
+        <v>3.2127099999999999E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B7">
+        <v>5</v>
+      </c>
+      <c r="C7">
+        <v>475.3</v>
+      </c>
+      <c r="D7">
+        <v>475.65</v>
+      </c>
+      <c r="E7">
+        <v>343.51799999999997</v>
+      </c>
+      <c r="F7">
+        <v>176.09700000000001</v>
+      </c>
+      <c r="G7">
+        <v>0.36272500000000002</v>
+      </c>
+      <c r="H7">
+        <v>3.2064700000000002E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B8">
+        <v>6</v>
+      </c>
+      <c r="C8">
+        <v>475.31200000000001</v>
+      </c>
+      <c r="D8">
+        <v>475.64600000000002</v>
+      </c>
+      <c r="E8">
+        <v>343.512</v>
+      </c>
+      <c r="F8">
+        <v>176.07499999999999</v>
+      </c>
+      <c r="G8">
+        <v>0.36281799999999997</v>
+      </c>
+      <c r="H8">
+        <v>3.2163299999999999E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B9">
+        <v>7</v>
+      </c>
+      <c r="C9">
+        <v>475.38200000000001</v>
+      </c>
+      <c r="D9">
+        <v>475.71699999999998</v>
+      </c>
+      <c r="E9">
+        <v>343.62599999999998</v>
+      </c>
+      <c r="F9">
+        <v>176.06299999999999</v>
+      </c>
+      <c r="G9">
+        <v>0.36292000000000002</v>
+      </c>
+      <c r="H9">
+        <v>3.2309299999999999E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B10">
+        <v>8</v>
+      </c>
+      <c r="C10">
+        <v>475.52199999999999</v>
+      </c>
+      <c r="D10">
+        <v>475.84899999999999</v>
+      </c>
+      <c r="E10">
+        <v>343.63200000000001</v>
+      </c>
+      <c r="F10">
+        <v>175.96899999999999</v>
+      </c>
+      <c r="G10">
+        <v>0.36304599999999998</v>
+      </c>
+      <c r="H10">
+        <v>3.2532600000000002E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B11">
+        <v>9</v>
+      </c>
+      <c r="C11">
+        <v>475.47300000000001</v>
+      </c>
+      <c r="D11">
+        <v>475.798</v>
+      </c>
+      <c r="E11">
+        <v>343.57400000000001</v>
+      </c>
+      <c r="F11">
+        <v>175.941</v>
+      </c>
+      <c r="G11">
+        <v>0.36258400000000002</v>
+      </c>
+      <c r="H11">
+        <v>3.2777000000000001E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B12">
+        <v>10</v>
+      </c>
+      <c r="C12">
+        <v>475.34699999999998</v>
+      </c>
+      <c r="D12">
+        <v>475.67</v>
+      </c>
+      <c r="E12">
+        <v>343.529</v>
+      </c>
+      <c r="F12">
+        <v>175.90299999999999</v>
+      </c>
+      <c r="G12">
+        <v>0.36273499999999997</v>
+      </c>
+      <c r="H12">
+        <v>3.2558200000000002E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B13">
+        <v>11</v>
+      </c>
+      <c r="C13">
+        <v>475.43599999999998</v>
+      </c>
+      <c r="D13">
+        <v>475.755</v>
+      </c>
+      <c r="E13">
+        <v>343.51</v>
+      </c>
+      <c r="F13">
+        <v>175.92699999999999</v>
+      </c>
+      <c r="G13">
+        <v>0.36260399999999998</v>
+      </c>
+      <c r="H13">
+        <v>3.2578799999999998E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B14">
+        <v>12</v>
+      </c>
+      <c r="C14">
+        <v>475.43</v>
+      </c>
+      <c r="D14">
+        <v>475.755</v>
+      </c>
+      <c r="E14">
+        <v>343.52600000000001</v>
+      </c>
+      <c r="F14">
+        <v>175.87</v>
+      </c>
+      <c r="G14">
+        <v>0.36316999999999999</v>
+      </c>
+      <c r="H14">
+        <v>3.2447900000000002E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B15">
+        <v>13</v>
+      </c>
+      <c r="C15">
+        <v>475.44400000000002</v>
+      </c>
+      <c r="D15">
+        <v>475.77100000000002</v>
+      </c>
+      <c r="E15">
+        <v>343.50099999999998</v>
+      </c>
+      <c r="F15">
+        <v>176.04499999999999</v>
+      </c>
+      <c r="G15">
+        <v>0.36301899999999998</v>
+      </c>
+      <c r="H15">
+        <v>3.2353399999999997E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B16">
+        <v>14</v>
+      </c>
+      <c r="C16">
+        <v>475.51600000000002</v>
+      </c>
+      <c r="D16">
+        <v>475.84699999999998</v>
+      </c>
+      <c r="E16">
+        <v>343.47300000000001</v>
+      </c>
+      <c r="F16">
+        <v>175.876</v>
+      </c>
+      <c r="G16">
+        <v>0.36296499999999998</v>
+      </c>
+      <c r="H16">
+        <v>3.2429100000000002E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B17">
+        <v>15</v>
+      </c>
+      <c r="C17">
+        <v>475.48399999999998</v>
+      </c>
+      <c r="D17">
+        <v>475.803</v>
+      </c>
+      <c r="E17">
+        <v>343.49700000000001</v>
+      </c>
+      <c r="F17">
+        <v>175.93600000000001</v>
+      </c>
+      <c r="G17">
+        <v>0.36278899999999997</v>
+      </c>
+      <c r="H17">
+        <v>3.2414400000000003E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B18">
+        <v>16</v>
+      </c>
+      <c r="C18">
+        <v>475.59699999999998</v>
+      </c>
+      <c r="D18">
+        <v>475.91800000000001</v>
+      </c>
+      <c r="E18">
+        <v>343.61399999999998</v>
+      </c>
+      <c r="F18">
+        <v>176.02600000000001</v>
+      </c>
+      <c r="G18">
+        <v>0.36255300000000001</v>
+      </c>
+      <c r="H18">
+        <v>3.2190200000000002E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B19">
+        <v>17</v>
+      </c>
+      <c r="C19">
+        <v>475.44799999999998</v>
+      </c>
+      <c r="D19">
+        <v>475.77499999999998</v>
+      </c>
+      <c r="E19">
+        <v>343.51400000000001</v>
+      </c>
+      <c r="F19">
+        <v>175.87899999999999</v>
+      </c>
+      <c r="G19">
+        <v>0.36227199999999998</v>
+      </c>
+      <c r="H19">
+        <v>3.2280799999999998E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B20">
+        <v>18</v>
+      </c>
+      <c r="C20">
+        <v>475.60700000000003</v>
+      </c>
+      <c r="D20">
+        <v>475.93599999999998</v>
+      </c>
+      <c r="E20">
+        <v>343.52100000000002</v>
+      </c>
+      <c r="F20">
+        <v>175.91300000000001</v>
+      </c>
+      <c r="G20">
+        <v>0.36220599999999997</v>
+      </c>
+      <c r="H20">
+        <v>3.2216099999999998E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B21">
+        <v>19</v>
+      </c>
+      <c r="C21">
+        <v>475.45600000000002</v>
+      </c>
+      <c r="D21">
+        <v>475.78500000000003</v>
+      </c>
+      <c r="E21">
+        <v>343.55500000000001</v>
+      </c>
+      <c r="F21">
+        <v>175.989</v>
+      </c>
+      <c r="G21">
+        <v>0.36219899999999999</v>
+      </c>
+      <c r="H21">
+        <v>3.2469999999999999E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B22">
+        <v>20</v>
+      </c>
+      <c r="C22">
+        <v>475.49099999999999</v>
+      </c>
+      <c r="D22">
+        <v>475.81799999999998</v>
+      </c>
+      <c r="E22">
+        <v>343.51299999999998</v>
+      </c>
+      <c r="F22">
+        <v>175.953</v>
+      </c>
+      <c r="G22">
+        <v>0.36247299999999999</v>
+      </c>
+      <c r="H22">
+        <v>3.2458399999999998E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B23">
+        <v>21</v>
+      </c>
+      <c r="C23">
+        <v>475.47399999999999</v>
+      </c>
+      <c r="D23">
+        <v>475.79899999999998</v>
+      </c>
+      <c r="E23">
+        <v>343.57400000000001</v>
+      </c>
+      <c r="F23">
+        <v>175.899</v>
+      </c>
+      <c r="G23">
+        <v>0.36206500000000003</v>
+      </c>
+      <c r="H23">
+        <v>3.2455499999999998E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B24">
+        <v>22</v>
+      </c>
+      <c r="C24">
+        <v>475.53199999999998</v>
+      </c>
+      <c r="D24">
+        <v>475.85399999999998</v>
+      </c>
+      <c r="E24">
+        <v>343.541</v>
+      </c>
+      <c r="F24">
+        <v>175.91499999999999</v>
+      </c>
+      <c r="G24">
+        <v>0.36268400000000001</v>
+      </c>
+      <c r="H24">
+        <v>3.2402300000000002E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B25">
+        <v>23</v>
+      </c>
+      <c r="C25">
+        <v>475.62099999999998</v>
+      </c>
+      <c r="D25">
+        <v>475.94099999999997</v>
+      </c>
+      <c r="E25">
+        <v>343.584</v>
+      </c>
+      <c r="F25">
+        <v>175.995</v>
+      </c>
+      <c r="G25">
+        <v>0.36233399999999999</v>
+      </c>
+      <c r="H25">
+        <v>3.2438799999999997E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B26">
+        <v>24</v>
+      </c>
+      <c r="C26">
+        <v>475.64</v>
+      </c>
+      <c r="D26">
+        <v>475.959</v>
+      </c>
+      <c r="E26">
+        <v>343.60599999999999</v>
+      </c>
+      <c r="F26">
+        <v>175.98099999999999</v>
+      </c>
+      <c r="G26">
+        <v>0.36259599999999997</v>
+      </c>
+      <c r="H26">
+        <v>3.25803E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B27">
+        <v>25</v>
+      </c>
+      <c r="C27">
+        <v>475.53800000000001</v>
+      </c>
+      <c r="D27">
+        <v>475.86</v>
+      </c>
+      <c r="E27">
+        <v>343.529</v>
+      </c>
+      <c r="F27">
+        <v>175.88900000000001</v>
+      </c>
+      <c r="G27">
+        <v>0.36243900000000001</v>
+      </c>
+      <c r="H27">
+        <v>3.2545400000000002E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B28">
+        <v>26</v>
+      </c>
+      <c r="C28">
+        <v>475.52499999999998</v>
+      </c>
+      <c r="D28">
+        <v>475.85500000000002</v>
+      </c>
+      <c r="E28">
+        <v>343.59100000000001</v>
+      </c>
+      <c r="F28">
+        <v>175.90199999999999</v>
+      </c>
+      <c r="G28">
+        <v>0.36257499999999998</v>
+      </c>
+      <c r="H28">
+        <v>3.2523299999999998E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B29">
+        <v>27</v>
+      </c>
+      <c r="C29">
+        <v>475.55200000000002</v>
+      </c>
+      <c r="D29">
+        <v>475.87599999999998</v>
+      </c>
+      <c r="E29">
+        <v>343.57799999999997</v>
+      </c>
+      <c r="F29">
+        <v>175.94499999999999</v>
+      </c>
+      <c r="G29">
+        <v>0.36272399999999999</v>
+      </c>
+      <c r="H29">
+        <v>3.23501E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B30">
+        <v>28</v>
+      </c>
+      <c r="C30">
+        <v>475.51</v>
+      </c>
+      <c r="D30">
+        <v>475.83699999999999</v>
+      </c>
+      <c r="E30">
+        <v>343.54899999999998</v>
+      </c>
+      <c r="F30">
+        <v>175.80099999999999</v>
+      </c>
+      <c r="G30">
+        <v>0.36263499999999999</v>
+      </c>
+      <c r="H30">
+        <v>3.2558799999999999E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B31">
+        <v>29</v>
+      </c>
+      <c r="C31">
+        <v>475.44400000000002</v>
+      </c>
+      <c r="D31">
+        <v>475.78</v>
+      </c>
+      <c r="E31">
+        <v>343.49299999999999</v>
+      </c>
+      <c r="F31">
+        <v>175.797</v>
+      </c>
+      <c r="G31">
+        <v>0.362514</v>
+      </c>
+      <c r="H31">
+        <v>3.25236E-2</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added tables to Readme.
</commit_message>
<xml_diff>
--- a/graphics.xlsx
+++ b/graphics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\opt\windows\Microsoft\VisualStudio\repos\CameraCalibration\QtFrontoParallel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C03AC03-1424-4A69-A989-631DEB058806}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B86D0056-D4EF-4ABE-92F5-02DE2D40881D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5568" activeTab="1" xr2:uid="{DFD5A370-DE3D-47F8-981C-568D4120CDD8}"/>
   </bookViews>
@@ -1293,94 +1293,94 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>0.37133899999999997</c:v>
+                  <c:v>0.29776900000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.36565399999999998</c:v>
+                  <c:v>0.29162199999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.36426900000000001</c:v>
+                  <c:v>0.28998200000000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.363541</c:v>
+                  <c:v>0.28955500000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.36338500000000001</c:v>
+                  <c:v>0.28958699999999998</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.36272500000000002</c:v>
+                  <c:v>0.28945199999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.36281799999999997</c:v>
+                  <c:v>0.28967700000000002</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.36292000000000002</c:v>
+                  <c:v>0.28950700000000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.36304599999999998</c:v>
+                  <c:v>0.28951199999999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.36258400000000002</c:v>
+                  <c:v>0.28916199999999997</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.36273499999999997</c:v>
+                  <c:v>0.28915200000000002</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.36260399999999998</c:v>
+                  <c:v>0.28919400000000001</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.36316999999999999</c:v>
+                  <c:v>0.288885</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.36301899999999998</c:v>
+                  <c:v>0.28920800000000002</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.36296499999999998</c:v>
+                  <c:v>0.28919600000000001</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.36278899999999997</c:v>
+                  <c:v>0.289273</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.36255300000000001</c:v>
+                  <c:v>0.28909899999999999</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.36227199999999998</c:v>
+                  <c:v>0.28904200000000002</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.36220599999999997</c:v>
+                  <c:v>0.289356</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.36219899999999999</c:v>
+                  <c:v>0.28943099999999999</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.36247299999999999</c:v>
+                  <c:v>0.28964600000000001</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.36206500000000003</c:v>
+                  <c:v>0.28941800000000001</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.36268400000000001</c:v>
+                  <c:v>0.28947000000000001</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.36233399999999999</c:v>
+                  <c:v>0.28947299999999998</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.36259599999999997</c:v>
+                  <c:v>0.289377</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.36243900000000001</c:v>
+                  <c:v>0.28930699999999998</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.36257499999999998</c:v>
+                  <c:v>0.28930099999999997</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.36272399999999999</c:v>
+                  <c:v>0.28923900000000002</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.36263499999999999</c:v>
+                  <c:v>0.28940300000000002</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.362514</c:v>
+                  <c:v>0.28945100000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1797,94 +1797,94 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>343.37299999999999</c:v>
+                  <c:v>350.85599999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>343.40499999999997</c:v>
+                  <c:v>350.77800000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>343.548</c:v>
+                  <c:v>350.803</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>343.488</c:v>
+                  <c:v>350.78899999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>343.49599999999998</c:v>
+                  <c:v>350.81799999999998</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>343.51799999999997</c:v>
+                  <c:v>350.79199999999997</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>343.512</c:v>
+                  <c:v>350.84199999999998</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>343.62599999999998</c:v>
+                  <c:v>350.78199999999998</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>343.63200000000001</c:v>
+                  <c:v>350.755</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>343.57400000000001</c:v>
+                  <c:v>350.81299999999999</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>343.529</c:v>
+                  <c:v>350.82499999999999</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>343.51</c:v>
+                  <c:v>350.83800000000002</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>343.52600000000001</c:v>
+                  <c:v>350.80599999999998</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>343.50099999999998</c:v>
+                  <c:v>350.81700000000001</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>343.47300000000001</c:v>
+                  <c:v>350.79500000000002</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>343.49700000000001</c:v>
+                  <c:v>350.68900000000002</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>343.61399999999998</c:v>
+                  <c:v>350.77499999999998</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>343.51400000000001</c:v>
+                  <c:v>350.71699999999998</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>343.52100000000002</c:v>
+                  <c:v>350.714</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>343.55500000000001</c:v>
+                  <c:v>350.75799999999998</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>343.51299999999998</c:v>
+                  <c:v>350.71899999999999</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>343.57400000000001</c:v>
+                  <c:v>350.66199999999998</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>343.541</c:v>
+                  <c:v>350.68099999999998</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>343.584</c:v>
+                  <c:v>350.69900000000001</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>343.60599999999999</c:v>
+                  <c:v>350.74200000000002</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>343.529</c:v>
+                  <c:v>350.75200000000001</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>343.59100000000001</c:v>
+                  <c:v>350.75200000000001</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>343.57799999999997</c:v>
+                  <c:v>350.74299999999999</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>343.54899999999998</c:v>
+                  <c:v>350.80599999999998</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>343.49299999999999</c:v>
+                  <c:v>350.71300000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1896,94 +1896,94 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>176.05199999999999</c:v>
+                  <c:v>178.87799999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>175.98699999999999</c:v>
+                  <c:v>179.00299999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>175.976</c:v>
+                  <c:v>178.99600000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>176.02</c:v>
+                  <c:v>179.077</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>175.99700000000001</c:v>
+                  <c:v>179.089</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>176.09700000000001</c:v>
+                  <c:v>179.06899999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>176.07499999999999</c:v>
+                  <c:v>179.001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>176.06299999999999</c:v>
+                  <c:v>178.99700000000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>175.96899999999999</c:v>
+                  <c:v>178.95099999999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>175.941</c:v>
+                  <c:v>178.94200000000001</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>175.90299999999999</c:v>
+                  <c:v>178.94399999999999</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>175.92699999999999</c:v>
+                  <c:v>178.99299999999999</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>175.87</c:v>
+                  <c:v>178.99100000000001</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>176.04499999999999</c:v>
+                  <c:v>178.93700000000001</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>175.876</c:v>
+                  <c:v>178.95599999999999</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>175.93600000000001</c:v>
+                  <c:v>178.947</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>176.02600000000001</c:v>
+                  <c:v>178.934</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>175.87899999999999</c:v>
+                  <c:v>178.904</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>175.91300000000001</c:v>
+                  <c:v>178.88900000000001</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>175.989</c:v>
+                  <c:v>178.87100000000001</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>175.953</c:v>
+                  <c:v>178.93</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>175.899</c:v>
+                  <c:v>178.90299999999999</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>175.91499999999999</c:v>
+                  <c:v>178.92</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>175.995</c:v>
+                  <c:v>178.89</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>175.98099999999999</c:v>
+                  <c:v>179.02</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>175.88900000000001</c:v>
+                  <c:v>178.95500000000001</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>175.90199999999999</c:v>
+                  <c:v>178.98500000000001</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>175.94499999999999</c:v>
+                  <c:v>178.91900000000001</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>175.80099999999999</c:v>
+                  <c:v>178.92400000000001</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>175.797</c:v>
+                  <c:v>178.95699999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5696,7 +5696,7 @@
   <dimension ref="B1:H31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P24" sqref="P24"/>
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5729,22 +5729,22 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>475.767</v>
+        <v>486.50099999999998</v>
       </c>
       <c r="D2">
-        <v>476.19</v>
+        <v>486.17399999999998</v>
       </c>
       <c r="E2">
-        <v>343.37299999999999</v>
+        <v>350.85599999999999</v>
       </c>
       <c r="F2">
-        <v>176.05199999999999</v>
+        <v>178.87799999999999</v>
       </c>
       <c r="G2">
-        <v>0.37133899999999997</v>
+        <v>0.29776900000000001</v>
       </c>
       <c r="H2">
-        <v>4.5352799999999999E-2</v>
+        <v>4.3717600000000002E-2</v>
       </c>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.3">
@@ -5752,22 +5752,22 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>475.36</v>
+        <v>486.56700000000001</v>
       </c>
       <c r="D3">
-        <v>475.75299999999999</v>
+        <v>486.19900000000001</v>
       </c>
       <c r="E3">
-        <v>343.40499999999997</v>
+        <v>350.77800000000002</v>
       </c>
       <c r="F3">
-        <v>175.98699999999999</v>
+        <v>179.00299999999999</v>
       </c>
       <c r="G3">
-        <v>0.36565399999999998</v>
+        <v>0.29162199999999999</v>
       </c>
       <c r="H3">
-        <v>3.5694700000000003E-2</v>
+        <v>3.4427699999999999E-2</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.3">
@@ -5775,22 +5775,22 @@
         <v>2</v>
       </c>
       <c r="C4">
-        <v>475.233</v>
+        <v>486.57400000000001</v>
       </c>
       <c r="D4">
-        <v>475.60199999999998</v>
+        <v>486.19400000000002</v>
       </c>
       <c r="E4">
-        <v>343.548</v>
+        <v>350.803</v>
       </c>
       <c r="F4">
-        <v>175.976</v>
+        <v>178.99600000000001</v>
       </c>
       <c r="G4">
-        <v>0.36426900000000001</v>
+        <v>0.28998200000000002</v>
       </c>
       <c r="H4">
-        <v>3.3199600000000003E-2</v>
+        <v>3.1148700000000001E-2</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.3">
@@ -5798,22 +5798,22 @@
         <v>3</v>
       </c>
       <c r="C5">
-        <v>475.20699999999999</v>
+        <v>486.65199999999999</v>
       </c>
       <c r="D5">
-        <v>475.55900000000003</v>
+        <v>486.25900000000001</v>
       </c>
       <c r="E5">
-        <v>343.488</v>
+        <v>350.78899999999999</v>
       </c>
       <c r="F5">
-        <v>176.02</v>
+        <v>179.077</v>
       </c>
       <c r="G5">
-        <v>0.363541</v>
+        <v>0.28955500000000001</v>
       </c>
       <c r="H5">
-        <v>3.2205299999999999E-2</v>
+        <v>3.0565700000000001E-2</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.3">
@@ -5821,22 +5821,22 @@
         <v>4</v>
       </c>
       <c r="C6">
-        <v>475.20699999999999</v>
+        <v>486.69299999999998</v>
       </c>
       <c r="D6">
-        <v>475.56</v>
+        <v>486.298</v>
       </c>
       <c r="E6">
-        <v>343.49599999999998</v>
+        <v>350.81799999999998</v>
       </c>
       <c r="F6">
-        <v>175.99700000000001</v>
+        <v>179.089</v>
       </c>
       <c r="G6">
-        <v>0.36338500000000001</v>
+        <v>0.28958699999999998</v>
       </c>
       <c r="H6">
-        <v>3.2127099999999999E-2</v>
+        <v>3.0590699999999998E-2</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.3">
@@ -5844,22 +5844,22 @@
         <v>5</v>
       </c>
       <c r="C7">
-        <v>475.3</v>
+        <v>486.721</v>
       </c>
       <c r="D7">
-        <v>475.65</v>
+        <v>486.31799999999998</v>
       </c>
       <c r="E7">
-        <v>343.51799999999997</v>
+        <v>350.79199999999997</v>
       </c>
       <c r="F7">
-        <v>176.09700000000001</v>
+        <v>179.06899999999999</v>
       </c>
       <c r="G7">
-        <v>0.36272500000000002</v>
+        <v>0.28945199999999999</v>
       </c>
       <c r="H7">
-        <v>3.2064700000000002E-2</v>
+        <v>3.0654600000000001E-2</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.3">
@@ -5867,22 +5867,22 @@
         <v>6</v>
       </c>
       <c r="C8">
-        <v>475.31200000000001</v>
+        <v>486.78300000000002</v>
       </c>
       <c r="D8">
-        <v>475.64600000000002</v>
+        <v>486.387</v>
       </c>
       <c r="E8">
-        <v>343.512</v>
+        <v>350.84199999999998</v>
       </c>
       <c r="F8">
-        <v>176.07499999999999</v>
+        <v>179.001</v>
       </c>
       <c r="G8">
-        <v>0.36281799999999997</v>
+        <v>0.28967700000000002</v>
       </c>
       <c r="H8">
-        <v>3.2163299999999999E-2</v>
+        <v>3.0684800000000002E-2</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.3">
@@ -5890,22 +5890,22 @@
         <v>7</v>
       </c>
       <c r="C9">
-        <v>475.38200000000001</v>
+        <v>486.86099999999999</v>
       </c>
       <c r="D9">
-        <v>475.71699999999998</v>
+        <v>486.47699999999998</v>
       </c>
       <c r="E9">
-        <v>343.62599999999998</v>
+        <v>350.78199999999998</v>
       </c>
       <c r="F9">
-        <v>176.06299999999999</v>
+        <v>178.99700000000001</v>
       </c>
       <c r="G9">
-        <v>0.36292000000000002</v>
+        <v>0.28950700000000001</v>
       </c>
       <c r="H9">
-        <v>3.2309299999999999E-2</v>
+        <v>3.0754400000000001E-2</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.3">
@@ -5913,22 +5913,22 @@
         <v>8</v>
       </c>
       <c r="C10">
-        <v>475.52199999999999</v>
+        <v>486.8</v>
       </c>
       <c r="D10">
-        <v>475.84899999999999</v>
+        <v>486.41800000000001</v>
       </c>
       <c r="E10">
-        <v>343.63200000000001</v>
+        <v>350.755</v>
       </c>
       <c r="F10">
-        <v>175.96899999999999</v>
+        <v>178.95099999999999</v>
       </c>
       <c r="G10">
-        <v>0.36304599999999998</v>
+        <v>0.28951199999999999</v>
       </c>
       <c r="H10">
-        <v>3.2532600000000002E-2</v>
+        <v>3.0664199999999999E-2</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.3">
@@ -5936,22 +5936,22 @@
         <v>9</v>
       </c>
       <c r="C11">
-        <v>475.47300000000001</v>
+        <v>486.82499999999999</v>
       </c>
       <c r="D11">
-        <v>475.798</v>
+        <v>486.45</v>
       </c>
       <c r="E11">
-        <v>343.57400000000001</v>
+        <v>350.81299999999999</v>
       </c>
       <c r="F11">
-        <v>175.941</v>
+        <v>178.94200000000001</v>
       </c>
       <c r="G11">
-        <v>0.36258400000000002</v>
+        <v>0.28916199999999997</v>
       </c>
       <c r="H11">
-        <v>3.2777000000000001E-2</v>
+        <v>3.04579E-2</v>
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.3">
@@ -5959,22 +5959,22 @@
         <v>10</v>
       </c>
       <c r="C12">
-        <v>475.34699999999998</v>
+        <v>486.76100000000002</v>
       </c>
       <c r="D12">
-        <v>475.67</v>
+        <v>486.38799999999998</v>
       </c>
       <c r="E12">
-        <v>343.529</v>
+        <v>350.82499999999999</v>
       </c>
       <c r="F12">
-        <v>175.90299999999999</v>
+        <v>178.94399999999999</v>
       </c>
       <c r="G12">
-        <v>0.36273499999999997</v>
+        <v>0.28915200000000002</v>
       </c>
       <c r="H12">
-        <v>3.2558200000000002E-2</v>
+        <v>3.0586800000000001E-2</v>
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.3">
@@ -5982,22 +5982,22 @@
         <v>11</v>
       </c>
       <c r="C13">
-        <v>475.43599999999998</v>
+        <v>486.81799999999998</v>
       </c>
       <c r="D13">
-        <v>475.755</v>
+        <v>486.44900000000001</v>
       </c>
       <c r="E13">
-        <v>343.51</v>
+        <v>350.83800000000002</v>
       </c>
       <c r="F13">
-        <v>175.92699999999999</v>
+        <v>178.99299999999999</v>
       </c>
       <c r="G13">
-        <v>0.36260399999999998</v>
+        <v>0.28919400000000001</v>
       </c>
       <c r="H13">
-        <v>3.2578799999999998E-2</v>
+        <v>3.0442899999999998E-2</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.3">
@@ -6005,22 +6005,22 @@
         <v>12</v>
       </c>
       <c r="C14">
-        <v>475.43</v>
+        <v>486.84500000000003</v>
       </c>
       <c r="D14">
-        <v>475.755</v>
+        <v>486.47500000000002</v>
       </c>
       <c r="E14">
-        <v>343.52600000000001</v>
+        <v>350.80599999999998</v>
       </c>
       <c r="F14">
-        <v>175.87</v>
+        <v>178.99100000000001</v>
       </c>
       <c r="G14">
-        <v>0.36316999999999999</v>
+        <v>0.288885</v>
       </c>
       <c r="H14">
-        <v>3.2447900000000002E-2</v>
+        <v>3.0373000000000001E-2</v>
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.3">
@@ -6028,22 +6028,22 @@
         <v>13</v>
       </c>
       <c r="C15">
-        <v>475.44400000000002</v>
+        <v>486.87</v>
       </c>
       <c r="D15">
-        <v>475.77100000000002</v>
+        <v>486.49900000000002</v>
       </c>
       <c r="E15">
-        <v>343.50099999999998</v>
+        <v>350.81700000000001</v>
       </c>
       <c r="F15">
-        <v>176.04499999999999</v>
+        <v>178.93700000000001</v>
       </c>
       <c r="G15">
-        <v>0.36301899999999998</v>
+        <v>0.28920800000000002</v>
       </c>
       <c r="H15">
-        <v>3.2353399999999997E-2</v>
+        <v>3.0482599999999999E-2</v>
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.3">
@@ -6051,22 +6051,22 @@
         <v>14</v>
       </c>
       <c r="C16">
-        <v>475.51600000000002</v>
+        <v>486.82400000000001</v>
       </c>
       <c r="D16">
-        <v>475.84699999999998</v>
+        <v>486.46300000000002</v>
       </c>
       <c r="E16">
-        <v>343.47300000000001</v>
+        <v>350.79500000000002</v>
       </c>
       <c r="F16">
-        <v>175.876</v>
+        <v>178.95599999999999</v>
       </c>
       <c r="G16">
-        <v>0.36296499999999998</v>
+        <v>0.28919600000000001</v>
       </c>
       <c r="H16">
-        <v>3.2429100000000002E-2</v>
+        <v>3.0372699999999999E-2</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.3">
@@ -6074,22 +6074,22 @@
         <v>15</v>
       </c>
       <c r="C17">
-        <v>475.48399999999998</v>
+        <v>486.80900000000003</v>
       </c>
       <c r="D17">
-        <v>475.803</v>
+        <v>486.44900000000001</v>
       </c>
       <c r="E17">
-        <v>343.49700000000001</v>
+        <v>350.68900000000002</v>
       </c>
       <c r="F17">
-        <v>175.93600000000001</v>
+        <v>178.947</v>
       </c>
       <c r="G17">
-        <v>0.36278899999999997</v>
+        <v>0.289273</v>
       </c>
       <c r="H17">
-        <v>3.2414400000000003E-2</v>
+        <v>3.0582000000000002E-2</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.3">
@@ -6097,22 +6097,22 @@
         <v>16</v>
       </c>
       <c r="C18">
-        <v>475.59699999999998</v>
+        <v>486.87299999999999</v>
       </c>
       <c r="D18">
-        <v>475.91800000000001</v>
+        <v>486.51100000000002</v>
       </c>
       <c r="E18">
-        <v>343.61399999999998</v>
+        <v>350.77499999999998</v>
       </c>
       <c r="F18">
-        <v>176.02600000000001</v>
+        <v>178.934</v>
       </c>
       <c r="G18">
-        <v>0.36255300000000001</v>
+        <v>0.28909899999999999</v>
       </c>
       <c r="H18">
-        <v>3.2190200000000002E-2</v>
+        <v>3.06945E-2</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.3">
@@ -6120,22 +6120,22 @@
         <v>17</v>
       </c>
       <c r="C19">
-        <v>475.44799999999998</v>
+        <v>486.81400000000002</v>
       </c>
       <c r="D19">
-        <v>475.77499999999998</v>
+        <v>486.45600000000002</v>
       </c>
       <c r="E19">
-        <v>343.51400000000001</v>
+        <v>350.71699999999998</v>
       </c>
       <c r="F19">
-        <v>175.87899999999999</v>
+        <v>178.904</v>
       </c>
       <c r="G19">
-        <v>0.36227199999999998</v>
+        <v>0.28904200000000002</v>
       </c>
       <c r="H19">
-        <v>3.2280799999999998E-2</v>
+        <v>3.07149E-2</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.3">
@@ -6143,22 +6143,22 @@
         <v>18</v>
       </c>
       <c r="C20">
-        <v>475.60700000000003</v>
+        <v>486.88099999999997</v>
       </c>
       <c r="D20">
-        <v>475.93599999999998</v>
+        <v>486.52300000000002</v>
       </c>
       <c r="E20">
-        <v>343.52100000000002</v>
+        <v>350.714</v>
       </c>
       <c r="F20">
-        <v>175.91300000000001</v>
+        <v>178.88900000000001</v>
       </c>
       <c r="G20">
-        <v>0.36220599999999997</v>
+        <v>0.289356</v>
       </c>
       <c r="H20">
-        <v>3.2216099999999998E-2</v>
+        <v>3.0840800000000002E-2</v>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.3">
@@ -6166,22 +6166,22 @@
         <v>19</v>
       </c>
       <c r="C21">
-        <v>475.45600000000002</v>
+        <v>486.83</v>
       </c>
       <c r="D21">
-        <v>475.78500000000003</v>
+        <v>486.46899999999999</v>
       </c>
       <c r="E21">
-        <v>343.55500000000001</v>
+        <v>350.75799999999998</v>
       </c>
       <c r="F21">
-        <v>175.989</v>
+        <v>178.87100000000001</v>
       </c>
       <c r="G21">
-        <v>0.36219899999999999</v>
+        <v>0.28943099999999999</v>
       </c>
       <c r="H21">
-        <v>3.2469999999999999E-2</v>
+        <v>3.05571E-2</v>
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.3">
@@ -6189,22 +6189,22 @@
         <v>20</v>
       </c>
       <c r="C22">
-        <v>475.49099999999999</v>
+        <v>486.86700000000002</v>
       </c>
       <c r="D22">
-        <v>475.81799999999998</v>
+        <v>486.50900000000001</v>
       </c>
       <c r="E22">
-        <v>343.51299999999998</v>
+        <v>350.71899999999999</v>
       </c>
       <c r="F22">
-        <v>175.953</v>
+        <v>178.93</v>
       </c>
       <c r="G22">
-        <v>0.36247299999999999</v>
+        <v>0.28964600000000001</v>
       </c>
       <c r="H22">
-        <v>3.2458399999999998E-2</v>
+        <v>3.0746800000000001E-2</v>
       </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.3">
@@ -6212,22 +6212,22 @@
         <v>21</v>
       </c>
       <c r="C23">
-        <v>475.47399999999999</v>
+        <v>486.74</v>
       </c>
       <c r="D23">
-        <v>475.79899999999998</v>
+        <v>486.38200000000001</v>
       </c>
       <c r="E23">
-        <v>343.57400000000001</v>
+        <v>350.66199999999998</v>
       </c>
       <c r="F23">
-        <v>175.899</v>
+        <v>178.90299999999999</v>
       </c>
       <c r="G23">
-        <v>0.36206500000000003</v>
+        <v>0.28941800000000001</v>
       </c>
       <c r="H23">
-        <v>3.2455499999999998E-2</v>
+        <v>3.06406E-2</v>
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.3">
@@ -6235,22 +6235,22 @@
         <v>22</v>
       </c>
       <c r="C24">
-        <v>475.53199999999998</v>
+        <v>486.85899999999998</v>
       </c>
       <c r="D24">
-        <v>475.85399999999998</v>
+        <v>486.49599999999998</v>
       </c>
       <c r="E24">
-        <v>343.541</v>
+        <v>350.68099999999998</v>
       </c>
       <c r="F24">
-        <v>175.91499999999999</v>
+        <v>178.92</v>
       </c>
       <c r="G24">
-        <v>0.36268400000000001</v>
+        <v>0.28947000000000001</v>
       </c>
       <c r="H24">
-        <v>3.2402300000000002E-2</v>
+        <v>3.0611699999999999E-2</v>
       </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.3">
@@ -6258,22 +6258,22 @@
         <v>23</v>
       </c>
       <c r="C25">
-        <v>475.62099999999998</v>
+        <v>486.923</v>
       </c>
       <c r="D25">
-        <v>475.94099999999997</v>
+        <v>486.56900000000002</v>
       </c>
       <c r="E25">
-        <v>343.584</v>
+        <v>350.69900000000001</v>
       </c>
       <c r="F25">
-        <v>175.995</v>
+        <v>178.89</v>
       </c>
       <c r="G25">
-        <v>0.36233399999999999</v>
+        <v>0.28947299999999998</v>
       </c>
       <c r="H25">
-        <v>3.2438799999999997E-2</v>
+        <v>3.0481100000000001E-2</v>
       </c>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.3">
@@ -6281,22 +6281,22 @@
         <v>24</v>
       </c>
       <c r="C26">
-        <v>475.64</v>
+        <v>486.923</v>
       </c>
       <c r="D26">
-        <v>475.959</v>
+        <v>486.56799999999998</v>
       </c>
       <c r="E26">
-        <v>343.60599999999999</v>
+        <v>350.74200000000002</v>
       </c>
       <c r="F26">
-        <v>175.98099999999999</v>
+        <v>179.02</v>
       </c>
       <c r="G26">
-        <v>0.36259599999999997</v>
+        <v>0.289377</v>
       </c>
       <c r="H26">
-        <v>3.25803E-2</v>
+        <v>3.0565800000000001E-2</v>
       </c>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.3">
@@ -6304,22 +6304,22 @@
         <v>25</v>
       </c>
       <c r="C27">
-        <v>475.53800000000001</v>
+        <v>486.834</v>
       </c>
       <c r="D27">
-        <v>475.86</v>
+        <v>486.47899999999998</v>
       </c>
       <c r="E27">
-        <v>343.529</v>
+        <v>350.75200000000001</v>
       </c>
       <c r="F27">
-        <v>175.88900000000001</v>
+        <v>178.95500000000001</v>
       </c>
       <c r="G27">
-        <v>0.36243900000000001</v>
+        <v>0.28930699999999998</v>
       </c>
       <c r="H27">
-        <v>3.2545400000000002E-2</v>
+        <v>3.05432E-2</v>
       </c>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.3">
@@ -6327,22 +6327,22 @@
         <v>26</v>
       </c>
       <c r="C28">
-        <v>475.52499999999998</v>
+        <v>486.899</v>
       </c>
       <c r="D28">
-        <v>475.85500000000002</v>
+        <v>486.541</v>
       </c>
       <c r="E28">
-        <v>343.59100000000001</v>
+        <v>350.75200000000001</v>
       </c>
       <c r="F28">
-        <v>175.90199999999999</v>
+        <v>178.98500000000001</v>
       </c>
       <c r="G28">
-        <v>0.36257499999999998</v>
+        <v>0.28930099999999997</v>
       </c>
       <c r="H28">
-        <v>3.2523299999999998E-2</v>
+        <v>3.04654E-2</v>
       </c>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.3">
@@ -6350,22 +6350,22 @@
         <v>27</v>
       </c>
       <c r="C29">
-        <v>475.55200000000002</v>
+        <v>486.91800000000001</v>
       </c>
       <c r="D29">
-        <v>475.87599999999998</v>
+        <v>486.565</v>
       </c>
       <c r="E29">
-        <v>343.57799999999997</v>
+        <v>350.74299999999999</v>
       </c>
       <c r="F29">
-        <v>175.94499999999999</v>
+        <v>178.91900000000001</v>
       </c>
       <c r="G29">
-        <v>0.36272399999999999</v>
+        <v>0.28923900000000002</v>
       </c>
       <c r="H29">
-        <v>3.23501E-2</v>
+        <v>3.0500699999999999E-2</v>
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.3">
@@ -6373,22 +6373,22 @@
         <v>28</v>
       </c>
       <c r="C30">
-        <v>475.51</v>
+        <v>486.83600000000001</v>
       </c>
       <c r="D30">
-        <v>475.83699999999999</v>
+        <v>486.47300000000001</v>
       </c>
       <c r="E30">
-        <v>343.54899999999998</v>
+        <v>350.80599999999998</v>
       </c>
       <c r="F30">
-        <v>175.80099999999999</v>
+        <v>178.92400000000001</v>
       </c>
       <c r="G30">
-        <v>0.36263499999999999</v>
+        <v>0.28940300000000002</v>
       </c>
       <c r="H30">
-        <v>3.2558799999999999E-2</v>
+        <v>3.05455E-2</v>
       </c>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.3">
@@ -6396,22 +6396,22 @@
         <v>29</v>
       </c>
       <c r="C31">
-        <v>475.44400000000002</v>
+        <v>486.80399999999997</v>
       </c>
       <c r="D31">
-        <v>475.78</v>
+        <v>486.44900000000001</v>
       </c>
       <c r="E31">
-        <v>343.49299999999999</v>
+        <v>350.71300000000002</v>
       </c>
       <c r="F31">
-        <v>175.797</v>
+        <v>178.95699999999999</v>
       </c>
       <c r="G31">
-        <v>0.362514</v>
+        <v>0.28945100000000001</v>
       </c>
       <c r="H31">
-        <v>3.25236E-2</v>
+        <v>3.0612299999999999E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added new image for description.
</commit_message>
<xml_diff>
--- a/graphics.xlsx
+++ b/graphics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\opt\windows\Microsoft\VisualStudio\repos\CameraCalibration\QtFrontoParallel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B86D0056-D4EF-4ABE-92F5-02DE2D40881D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B65218AC-2944-498A-8839-F64A58405BA2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5568" activeTab="1" xr2:uid="{DFD5A370-DE3D-47F8-981C-568D4120CDD8}"/>
   </bookViews>
@@ -4967,7 +4967,7 @@
   <dimension ref="B1:H31"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="H1" sqref="B1:H1"/>
+      <selection activeCell="Q16" sqref="Q16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>